<commit_message>
Added week type field to database.
</commit_message>
<xml_diff>
--- a/usb-database-design.xlsx
+++ b/usb-database-design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="191">
   <si>
     <t>Field</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>Week type</t>
+  </si>
+  <si>
+    <t>weektype</t>
   </si>
   <si>
     <t>Reserve</t>
@@ -1055,10 +1061,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2446,6 +2452,23 @@
         <v>63</v>
       </c>
       <c r="E80" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="0" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2465,10 +2488,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2487,11 +2510,11 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F1" s="4"/>
     </row>
@@ -2508,7 +2531,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2613,7 +2636,7 @@
         <v>Team Leader</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -2630,7 +2653,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,7 +2749,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C17" s="14"/>
       <c r="E17" s="15" t="str">
@@ -2820,7 +2843,7 @@
         <v>Eve Phone</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F23" s="17"/>
     </row>
@@ -2923,13 +2946,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="19" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C32" s="22"/>
       <c r="E32" s="18" t="s">
@@ -2941,7 +2964,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>64</v>
@@ -2960,7 +2983,7 @@
         <v>86</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E34" s="7" t="str">
         <f aca="false">Sheet1!C3</f>
@@ -2993,26 +3016,26 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C37" s="25" t="str">
         <f aca="false">Sheet1!B46</f>
         <v>Liability Forms</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F37" s="27"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C38" s="25" t="str">
         <f aca="false">Sheet1!B47</f>
@@ -3029,10 +3052,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C39" s="25" t="str">
         <f aca="false">Sheet1!B48</f>
@@ -3052,10 +3075,10 @@
         <v>8</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E40" s="5" t="str">
         <f aca="false">Sheet1!C21</f>
@@ -3071,7 +3094,7 @@
         <v>16</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C41" s="25" t="str">
         <f aca="false">Sheet1!B49</f>
@@ -3091,10 +3114,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E42" s="5" t="str">
         <f aca="false">Sheet1!C27</f>
@@ -3117,7 +3140,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="32" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C44" s="33"/>
       <c r="E44" s="7" t="str">
@@ -3149,7 +3172,7 @@
         <v>Church name</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F46" s="35"/>
     </row>
@@ -3200,70 +3223,80 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="7" t="str">
+      <c r="E50" s="5" t="str">
         <f aca="false">Sheet1!C80</f>
         <v>end</v>
       </c>
-      <c r="F50" s="8" t="str">
+      <c r="F50" s="6" t="str">
         <f aca="false">Sheet1!B80</f>
         <v>End Date</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C51" s="38"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="39"/>
-      <c r="B52" s="5" t="str">
-        <f aca="false">Sheet1!C17</f>
-        <v>wkcap</v>
-      </c>
-      <c r="C52" s="6" t="str">
-        <f aca="false">Sheet1!B17</f>
-        <v>Weekly Cap</v>
-      </c>
+      <c r="E51" s="7" t="str">
+        <f aca="false">Sheet1!C81</f>
+        <v>weektype</v>
+      </c>
+      <c r="F51" s="8" t="str">
+        <f aca="false">Sheet1!B81</f>
+        <v>Week type</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="38"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="39"/>
       <c r="B53" s="5" t="str">
-        <f aca="false">Sheet1!C18</f>
-        <v>wkmax</v>
+        <f aca="false">Sheet1!C17</f>
+        <v>wkcap</v>
       </c>
       <c r="C53" s="6" t="str">
-        <f aca="false">Sheet1!B18</f>
-        <v>Weekly Max</v>
+        <f aca="false">Sheet1!B17</f>
+        <v>Weekly Cap</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="39"/>
       <c r="B54" s="5" t="str">
+        <f aca="false">Sheet1!C18</f>
+        <v>wkmax</v>
+      </c>
+      <c r="C54" s="6" t="str">
+        <f aca="false">Sheet1!B18</f>
+        <v>Weekly Max</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="39"/>
+      <c r="B55" s="5" t="str">
         <f aca="false">Sheet1!C19</f>
         <v>rvmax</v>
       </c>
-      <c r="C54" s="6" t="str">
+      <c r="C55" s="6" t="str">
         <f aca="false">Sheet1!B19</f>
         <v>Max RV Slips</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="39"/>
-      <c r="B55" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="39"/>
-      <c r="B56" s="7" t="str">
+      <c r="B56" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="39"/>
+      <c r="B57" s="7" t="str">
         <f aca="false">Sheet1!C20</f>
         <v>apmax</v>
       </c>
-      <c r="C56" s="8" t="str">
+      <c r="C57" s="8" t="str">
         <f aca="false">Sheet1!B20</f>
         <v>Max Apartments</v>
       </c>

</xml_diff>